<commit_message>
add material design and hint card
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skato/Dropbox/ghq/github.com/sosuke-k/examination-electron/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skato/Dropbox/ghq/github.com/sosuke-k/collecting-electron/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6341D620-BA4F-C948-B62A-49CF31E70A11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797C2552-998D-D840-B7E3-D86EA743B4E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{F3924A9C-01AD-674B-B1DE-3DB21FCD4698}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Q</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>登る人のスペルを答えないさい</t>
+  </si>
+  <si>
+    <t>HINT</t>
+  </si>
+  <si>
+    <t>c****er</t>
+  </si>
+  <si>
+    <t>s****er</t>
   </si>
 </sst>
 </file>
@@ -394,36 +403,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543D0292-03F7-B645-B5FA-E8243CE5094E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>